<commit_message>
fix: remove header option
</commit_message>
<xml_diff>
--- a/excel/test/demo.xlsx
+++ b/excel/test/demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/honorluo/py-toolkit/excel/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBD9CD2-0A83-DF41-8271-D8E891D921BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609F1D8-8538-C945-821B-FD4AF036E772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>排名</t>
   </si>
@@ -34,21 +34,6 @@
     <t>积分</t>
   </si>
   <si>
-    <t>老板</t>
-  </si>
-  <si>
-    <t>rank</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>session</t>
-  </si>
-  <si>
-    <t>score</t>
-  </si>
-  <si>
     <t>BOSS</t>
   </si>
   <si>
@@ -58,33 +43,26 @@
     <t>Jim</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>国际米兰</t>
   </si>
   <si>
     <t>ZKY</t>
-  </si>
-  <si>
-    <t>尤文图斯</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -102,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -110,30 +88,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -436,99 +396,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F5"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>43</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>